<commit_message>
feat: apply italic and bold font changes to styles3.xlsx
</commit_message>
<xml_diff>
--- a/Chap14_Excel-Spreadsheets/styles3.xlsx
+++ b/Chap14_Excel-Spreadsheets/styles3.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
     </font>
     <font>
       <i val="1"/>
@@ -50,9 +54,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -418,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +434,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Hello, world!</t>
+          <t>Bold Times New Roman</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>24 pt Italic</t>
         </is>
       </c>
     </row>

</xml_diff>